<commit_message>
finalizado a inportação de 20 locais para dentro do projeto
</commit_message>
<xml_diff>
--- a/assets/xlsx/locais.xlsx
+++ b/assets/xlsx/locais.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\Área de Trabalho\Website_Turismo_Proz_1\Website_Turismo_Proz_1\assets\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17BB0A76-F4DB-4BAE-B11E-545C853C0F58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56BB0DFA-BADD-4673-878F-F7FB38C5FB05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="106">
   <si>
     <t>id</t>
   </si>
@@ -95,13 +95,269 @@
   </si>
   <si>
     <t>https://source.unsplash.com/random/560x400/?Florianopolis+SC;https://source.unsplash.com/random/560x400/?Florianopolis+SC;https://source.unsplash.com/random/560x400/?Florianopolis+SC;https://source.unsplash.com/random/560x400/?Florianopolis+SC;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Gramado - RS</t>
+  </si>
+  <si>
+    <t>https://source.unsplash.com/random/560x400/?Gramado+RS;https://source.unsplash.com/random/560x400/?Gramado+RS;https://source.unsplash.com/random/560x400/?Gramado+RS;https://source.unsplash.com/random/560x400/?Gramado+RS;</t>
+  </si>
+  <si>
+    <t>Gramado é uma encantadora cidade localizada na Serra Gaúcha, no estado do Rio Grande do Sul. Conhecida por sua atmosfera europeia, paisagens deslumbrantes e clima ameno, é um destino turístico popular no Brasil. Com sua arquitetura charmosa, culinária deliciosa e uma série de atrações, Gramado oferece uma experiência única aos seus visitantes.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lago Negro: O Lago Negro é um dos cartões-postais mais famosos de Gramado;Rua Coberta: A Rua Coberta é um dos principais pontos de encontro em Gramado;Mini Mundo: O Mini Mundo é uma atração fascinante em Gramado;Snowland: O Snowland é o primeiro parque de neve indoor das Américas e uma das principais atrações de Gramado. </t>
+  </si>
+  <si>
+    <t>Carro particular: Gramado é uma cidade que oferece boas condições para a circulação de veículos. Para quem deseja mais autonomia e comodidade, alugar um carro pode ser uma opção interessante, permitindo explorar os arredores e visitar os pontos turísticos da região no seu próprio ritmo; Táxi ou Uber: Tanto os táxis quanto o serviço de transporte por aplicativo estão disponíveis em Gramado. São opções práticas para se locomover pela cidade, especialmente para visitar pontos turísticos específicos ou quando não se deseja se preocupar com estacionamento; Ônibus turístico: Gramado possui um ônibus turístico que percorre os principais pontos da cidade. É uma opção conveniente para conhecer os pontos turísticos mais populares, com a vantagem de ter um guia fornecendo informações sobre cada local;Caminhadas: Gramado é uma cidade que pode ser facilmente explorada a pé. Muitos pontos turísticos estão próximos uns dos outros, permitindo que os visitantes desfrutem de agradáveis caminhadas pelas ruas charmosas da cidade.</t>
+  </si>
+  <si>
+    <t>Bonito - MS</t>
+  </si>
+  <si>
+    <t>https://source.unsplash.com/random/560x400/?Bonito+MS;https://source.unsplash.com/random/560x400/?Bonito+MS;https://source.unsplash.com/random/560x400/?Bonito+MS;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bonito é um verdadeiro paraíso natural localizado no estado do Mato Grosso do Sul, no Brasil. Conhecida por suas águas cristalinas, rios, cavernas e uma rica diversidade de fauna e flora, a cidade atrai turistas de todo o mundo em busca de aventura e contato com a natureza. Com uma infraestrutura bem desenvolvida para o ecoturismo, Bonito oferece experiências únicas e preservadas para os amantes da natureza.
+</t>
+  </si>
+  <si>
+    <t>Gruta do Lago Azul: A Gruta do Lago Azul é uma das atrações mais famosas de Bonito;Rio da Prata: O passeio pelo Rio da Prata é uma experiência imperdível em Bonito;Abismo Anhumas: O Abismo Anhumas é uma aventura emocionante para os amantes de atividades radicais;Flutuação no Rio Sucuri: O Rio Sucuri oferece uma experiência de flutuação inesquecível.</t>
+  </si>
+  <si>
+    <t>Carro particular: A forma mais comum de se locomover em Bonito é de carro particular. A cidade conta com boas estradas e é possível alugar um veículo para explorar os diversos pontos turísticos da região e as atrações naturais ao redor;Transporte em grupo: Muitas agências de turismo em Bonito oferecem serviços de transporte em grupo, especialmente para os passeios mais populares. Os visitantes podem contratar pacotes que incluem o transporte de ida e volta dos hotéis para as atrações turísticas, facilitando o deslocamento;Bicicleta: Bonito possui uma infraestrutura favorável para o uso de bicicletas. Alguns hotéis e pousadas disponibilizam bicicletas para seus hóspedes, permitindo que eles se desloquem de forma sustentável e apreciem a cidade e seus arredores em um ritmo mais tranquilo.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Paraty - RJ</t>
+  </si>
+  <si>
+    <t>https://source.unsplash.com/random/560x400/?Paraty+RJ;https://source.unsplash.com/random/560x400/?Paraty+RJ;https://source.unsplash.com/random/560x400/?Paraty+RJ;</t>
+  </si>
+  <si>
+    <t>Paraty é uma charmosa cidade histórica localizada no estado do Rio de Janeiro, no Brasil. Com sua arquitetura colonial preservada, ruas de pedra e localização privilegiada entre a serra e o mar, Paraty encanta os visitantes com seu clima tranquilo e suas belezas naturais. Além do patrimônio histórico, a cidade também é conhecida por suas praias paradisíacas e pela vasta oferta de passeios de barco e trilhas.</t>
+  </si>
+  <si>
+    <t>Centro Histórico de Paraty: O centro histórico de Paraty é uma verdadeira viagem ao passado;Passeios de barco pela Baía de Paraty: Os passeios de barco pela Baía de Paraty são uma das atrações mais populares da região;Trilhas e cachoeiras: A região de Paraty oferece diversas trilhas e cachoeiras para os amantes da natureza;Praias de Paraty: Paraty abriga praias de tirar o fôlego, tanto na própria cidade quanto em seus arredores</t>
+  </si>
+  <si>
+    <t>Caminhadas: Paraty é uma cidade compacta e muito charmosa, sendo possível explorar grande parte de suas atrações a pé. Caminhar pelas ruas do centro histórico e desfrutar da atmosfera tranquila é uma experiência encantadora; Táxi: Para trajetos mais longos ou para visitar praias e cachoeiras distantes do centro de Paraty, é possível utilizar serviços de táxi, que oferecem transporte de forma conveniente e confortável; Passeios de barco: Uma das melhores formas de se locomover e explorar as belezas naturais de Paraty é por meio de passeios de barco. Há diversas opções de passeios que percorrem as ilhas, praias e piscinas naturais, permitindo aos visitantes desfrutar das paisagens deslumbrantes da região</t>
+  </si>
+  <si>
+    <t>Manaus - AM</t>
+  </si>
+  <si>
+    <t>https://source.unsplash.com/random/560x400/?Manaus+AM;https://source.unsplash.com/random/560x400/?Manaus+AM;https://source.unsplash.com/random/560x400/?Manaus+AM;</t>
+  </si>
+  <si>
+    <t>Manaus, a capital do estado do Amazonas, é uma cidade fascinante localizada no coração da Amazônia brasileira. Conhecida por sua biodiversidade, cultura rica e herança histórica, Manaus é o ponto de partida ideal para explorar a maior floresta tropical do mundo. Com seu clima tropical e paisagens deslumbrantes, a cidade oferece uma experiência única aos turistas, que podem mergulhar na natureza exuberante e descobrir a história e a cultura da região.</t>
+  </si>
+  <si>
+    <t>Teatro Amazonas: O Teatro Amazonas é um dos ícones mais famosos de Manaus;Encontro das Águas: O Encontro das Águas é um espetáculo natural impressionante, onde as águas escuras do Rio Negro se encontram com as águas barrentas do Rio Solimões, formando o Rio Amazonas;Museu do Seringal Vila Paraíso: Localizado a aproximadamente 30 minutos de Manaus, o Museu do Seringal Vila Paraíso oferece aos visitantes a oportunidade de aprender sobre o período do ciclo da borracha na Amazônia;Passeio de barco pelo Rio Negro: Uma das melhores maneiras de explorar a Amazônia é fazer um passeio de barco pelo Rio Negro.</t>
+  </si>
+  <si>
+    <t>Barco regional: Para chegar a Manaus, uma opção interessante é fazer a viagem de barco regional a partir de cidades próximas, como Belém. Essa é uma experiência única, onde os turistas podem apreciar as paisagens ao longo do Rio Amazonas e vivenciar a cultura ribeirinha;Ônibus: Em Manaus, o sistema de transporte público conta com uma rede de ônibus que cobre a maior parte da cidade. É uma opção econômica para se deslocar dentro da cidade, principalmente para visitar os pontos turísticos mais próximos;Táxi e aplicativos de transporte: Táxis e aplicativos de transporte, como Uber, estão disponíveis em Manaus e são uma opção conveniente para se locomover pela cidade, especialmente</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Foz do Iguaçu - PR</t>
+  </si>
+  <si>
+    <t>Foz do Iguaçu, localizada no estado do Paraná, é uma cidade famosa por abrigar uma das mais impressionantes maravilhas naturais do mundo: as Cataratas do Iguaçu. Além das espetaculares quedas d'água, Foz do Iguaçu é uma cidade multicultural, marcada pela diversidade étnica e pela rica biodiversidade da região. Com uma localização estratégica na tríplice fronteira entre Brasil, Paraguai e Argentina, a cidade oferece aos turistas uma experiência única, com paisagens deslumbrantes e atrações imperdíveis.</t>
+  </si>
+  <si>
+    <t>Cataratas do Iguaçu: As Cataratas do Iguaçu são o principal atrativo de Foz do Iguaçu e uma das maravilhas naturais mais espetaculares do mundo;Parque Nacional do Iguaçu: O Parque Nacional do Iguaçu é uma área de preservação ambiental que abriga as Cataratas do Iguaçu;Marco das Três Fronteiras: O Marco das Três Fronteiras é um ponto turístico emblemático em Foz do Iguaçu, localizado na fronteira entre Brasil, Paraguai e Argentina;Itaipu Binacional: A Usina Hidrelétrica de Itaipu é uma das maiores do mundo e um importante marco na engenharia</t>
+  </si>
+  <si>
+    <t>Ônibus: Foz do Iguaçu possui um sistema de transporte público que abrange a cidade e seus principais pontos turísticos. Os ônibus são uma opção econômica para se deslocar pela região, com linhas que conectam os principais atrativos;Táxi e aplicativos de transporte: Táxis e aplicativos de transporte, como Uber, estão disponíveis em Foz do Iguaçu e oferecem conveniência e conforto para os deslocamentos, especialmente para quem prefere um serviço mais privativo ou precisa se deslocar em horários específicos.</t>
+  </si>
+  <si>
+    <t>Ouro Preto - MG</t>
+  </si>
+  <si>
+    <t>https://source.unsplash.com/random/560x400/?foz+do+Iguaçu+PR;https://source.unsplash.com/random/560x400/?foz+do+Iguaçu+PR;https://source.unsplash.com/random/560x400/?foz+do+Iguaçu+PR;</t>
+  </si>
+  <si>
+    <t>https://source.unsplash.com/random/560x400/?Ouro+Preto+MG;https://source.unsplash.com/random/560x400/?Ouro+Preto+MG;https://source.unsplash.com/random/560x400/?Ouro+Preto+MG;</t>
+  </si>
+  <si>
+    <t>Ouro Preto é uma cidade histórica localizada no estado de Minas Gerais, no Brasil. Reconhecida como Patrimônio Mundial pela UNESCO, a cidade preserva a rica herança do período colonial brasileiro. Com suas ladeiras de paralelepípedos, igrejas barrocas, museus e paisagens encantadoras, Ouro Preto atrai visitantes de todo o mundo em busca de cultura, história e beleza arquitetônica. Além disso, a cidade é conhecida pela sua vibrante vida estudantil, pois abriga uma importante universidade.</t>
+  </si>
+  <si>
+    <t>Igreja de São Francisco de Assis: A Igreja de São Francisco de Assis é uma das mais famosas e impressionantes igrejas de Ouro Preto;Museu da Inconfidência: O Museu da Inconfidência está localizado na antiga Casa de Câmara e Cadeia de Ouro Preto;Praça Tiradentes: A Praça Tiradentes é o coração de Ouro Preto, onde a cidade começou a ser construída;Mina da Passagem: A Mina da Passagem é uma antiga mina de ouro que hoje é aberta para visitação turística.</t>
+  </si>
+  <si>
+    <t>Caminhadas: Ouro Preto é uma cidade compacta e muitas das atrações turísticas estão localizadas próximas umas das outras. Caminhar pelas ruas íngremes e históricas de Ouro Preto é uma maneira agradável de explorar a cidade, permitindo apreciar a arquitetura colonial e descobrir cantinhos encantadores;Ônibus local: Ouro Preto possui um sistema de transporte público que conecta diferentes partes da cidade. Os ônibus locais são uma opção conveniente e econômica para se deslocar entre os principais pontos turísticos e bairros;Táxi: Táxis estão disponíveis em Ouro Preto e podem ser uma opção conveniente para se deslocar pela cidade, especialmente em trajetos mais curtos ou quando se deseja mais comodidade;Carro alugado: Para aqueles que preferem mais autonomia e flexibilidade, alugar um carro pode ser uma opção interessante em Ouro Preto. Isso permite explorar a cidade e seus arredores no seu próprio ritmo, visitando lugares mais afastados e aproveitando a comodidade de ter um veículo próprio;Bicicleta: Ouro Preto possui uma topografia montanhosa, mas também oferece opções de aluguel de bicicletas para os visitantes que desejam explorar a cidade de forma mais ativa. Existem trilhas e rotas cênicas que podem ser percorridas de bicicleta, proporcionando uma experiência diferente e contato mais próximo com a natureza.</t>
+  </si>
+  <si>
+    <t>Jericoacoara - CE</t>
+  </si>
+  <si>
+    <t>https://source.unsplash.com/random/560x400/?Jericoacoara+CE;https://source.unsplash.com/random/560x400/?Jericoacoara+CE;https://source.unsplash.com/random/560x400/?Jericoacoara+CE;</t>
+  </si>
+  <si>
+    <t>Jericoacoara, carinhosamente conhecida como "Jeri", é uma charmosa vila de pescadores localizada no litoral do estado do Ceará, no nordeste do Brasil. Com suas praias paradisíacas, dunas de areia branca, lagoas cristalinas e paisagens deslumbrantes, Jericoacoara é um destino turístico popular, atraindo visitantes em busca de relaxamento, aventura e contato com a natureza. Além de suas belezas naturais, Jeri oferece uma atmosfera descontraída, com ruas de areia, restaurantes aconchegantes, lojinhas de artesanato e uma vida noturna animada.</t>
+  </si>
+  <si>
+    <t>Duna do Pôr do Sol: Um dos momentos mais esperados em Jericoacoara é o pôr do sol;Praia de Jericoacoara: A praia principal de Jericoacoara é um verdadeiro cartão-postal;Lagoa do Paraíso: A Lagoa do Paraíso é um verdadeiro paraíso na terra;Pedra Furada: Um dos pontos turísticos mais emblemáticos de Jericoacoara é a Pedra Furada.</t>
+  </si>
+  <si>
+    <t>Caminhadas: Jericoacoara é uma vila compacta e a maioria das atrações turísticas estão localizadas a uma curta distância uma da outra. Caminhar pelas ruas de areia é a forma mais comum de se deslocar dentro da vila, permitindo explorar o local no seu próprio ritmo;Bugue e Jardineira: O bugue e a jardineira são meios de transporte típicos de Jericoacoara. São veículos ideais para explorar as dunas, lagoas e praias da região. Os bugueiros e motoristas de jardineiras são experientes e conhecem bem a região, levando os visitantes em passeios emocionantes pelas paisagens naturais de Jeri;Táxi: Táxis também estão disponíveis em Jericoacoara, oferecendo uma opção conveniente para se deslocar pela vila e seus arredores. É importante combinar o preço da corrida com o taxista antes de embarcar;Quadriciclos: Para quem busca mais aventura, alugar um quadriciclo pode ser uma opção emocionante. Os quadriciclos permitem explorar áreas mais afastadas e são perfeitos para quem deseja percorrer as dunas de forma mais rápida e divertida;Bicicleta: Jericoacoara é uma vila com ótima infraestrutura para ciclistas. Alugar uma bicicleta é uma maneira agradável de se locomover pela vila e explorar as praias e lagoas nos arredores. Existem várias lojas de aluguel de bicicletas disponíveis na região.</t>
+  </si>
+  <si>
+    <t>Olinda- PE</t>
+  </si>
+  <si>
+    <t>https://source.unsplash.com/random/560x400/?Olinda+PE;https://source.unsplash.com/random/560x400/?Olinda+PE;https://source.unsplash.com/random/560x400/?Olinda+PE;</t>
+  </si>
+  <si>
+    <t>Olinda é uma cidade histórica e culturalmente rica localizada no estado de Pernambuco, no nordeste do Brasil. Fundada em 1535, é considerada Patrimônio Cultural da Humanidade pela UNESCO devido ao seu centro histórico bem preservado, casario colorido, igrejas centenárias e festividades populares. Olinda é famosa por suas ruas de paralelepípedos, ladeiras íngremes, manifestações artísticas e pela alegria contagiante de seu povo. É um destino encantador que oferece uma combinação única de história, arte, religião e beleza natural.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Centro Histórico de Olinda: O centro histórico é o coração de Olinda e abriga diversas atrações imperdíveis, como a Catedral da Sé, o Convento de São Francisco, a Igreja da Misericórdia e o Alto da Sé, onde é possível apreciar uma vista panorâmica deslumbrante da cidade;Mercado da Ribeira: O Mercado da Ribeira é um local vibrante e repleto de cultura;Museu de Arte Contemporânea de Olinda (MAC): Localizado no antigo Convento de São Francisco, o MAC é um importante centro ultural em Olinda;Praia de Olinda: Apesar de não ser conhecida por suas praias, Olinda possui uma costa encantadora que vale a pena explorar. </t>
+  </si>
+  <si>
+    <t>Caminhadas: A melhor forma de explorar o centro histórico de Olinda é a pé. As ruas estreitas e as ladeiras íngremes são facilmente percorridas a pé, permitindo que os visitantes apreciem a arquitetura, as igrejas e a atmosfera única da cidade;Táxi: Táxis estão disponíveis em Olinda e são uma opção conveniente para se deslocar dentro da cidade e também para chegar a outros destinos próximos;Ônibus: O transporte público de ônibus é uma opção acessível para se deslocar entre Olinda e outras cidades da região, como Recife. Existem linhas de ônibus que conectam os principais pontos turísticos das duas cidades;Carro particular: Para aqueles que desejam mais autonomia e flexibilidade, alugar um carro particular é uma opção viável. É importante lembrar que, devido às ruas estreitas e à falta de estacionamento, pode ser desafiador encontrar vagas próximas aos pontos turísticos mais movimentados;Transporte por aplicativo: Os serviços de transporte por aplicativo, como Uber e 99, também estão disponíveis em Olinda e podem ser uma opção conveniente para se locomover na cidade e região.</t>
+  </si>
+  <si>
+    <t>Curitiba - PR</t>
+  </si>
+  <si>
+    <t>https://source.unsplash.com/random/560x400/?Curitiba+PR;https://source.unsplash.com/random/560x400/?Curitiba+PR;https://source.unsplash.com/random/560x400/?Curitiba+PR;</t>
+  </si>
+  <si>
+    <t>Curitiba é a capital do estado do Paraná, localizada na região sul do Brasil. Conhecida por sua qualidade de vida, planejamento urbano e cultura vibrante, a cidade é um destino turístico encantador. Curitiba oferece uma mistura única de natureza exuberante, arquitetura moderna, parques bem cuidados e uma cena cultural diversificada. Com uma infraestrutura eficiente, a cidade é famosa por suas atrações turísticas, gastronomia deliciosa, eventos culturais e o famoso sistema de transporte público.</t>
+  </si>
+  <si>
+    <t>Jardim Botânico: O Jardim Botânico de Curitiba é um dos pontos turísticos mais icônicos da cidade;Ópera de Arame: Localizada em meio a um lago e cercada de mata nativa, a Ópera de Arame é um teatro de estrutura tubular e teto transparente;Parque Tanguá: O Parque Tanguá é um lugar encantador que combina natureza, lagos, cachoeiras e belos jardins;Museu Oscar Niemeyer: Conhecido como "Museu do Olho" devido ao seu formato característico, o Museu Oscar Niemeyer é uma obra-prima arquitetônica.</t>
+  </si>
+  <si>
+    <t>Sistema de Transporte Integrado de Curitiba (Rede Integrada de Transporte - RIT): Curitiba é famosa por seu sistema de transporte público eficiente e bem planejado. O RIT inclui ônibus convencionais, chamados de "biarticulados" e "expressos", que conectam diferentes regiões da cidade. É uma opção conveniente e acessível para se deslocar pelos principais pontos turísticos e bairros de Curitiba;Táxi e transporte por aplicativo: Táxis e serviços de transporte por aplicativo, como Uber e 99, também estão disponíveis em Curitiba. São opções práticas para viagens mais curtas ou para se deslocar de forma mais privativa;Bicicleta: Curitiba possui uma extensa rede de ciclovias e ciclofaixas, o que torna a cidade muito amigável para os ciclistas. É possível alugar bicicletas em diversos pontos da cidade e explorar as áreas verdes e os parques de Curitiba de forma sustentável e saudável;Carro particular: Para aqueles que preferem mais autonomia e flexibilidade, alugar um carro particular pode ser uma opção. Curitiba possui boas vias e estacionamentos, o que facilita o deslocamento de carro pela cidade e a visita a destinos próximos;Caminhadas: Curitiba é uma cidade planejada, com calçadas amplas e agradáveis, tornando-se um ótimo local para caminhar. Muitos pontos turísticos estão próximos uns dos outros, permitindo que os visitantes explorem a cidade a pé e apreciem a arquitetura, os parques e as áreas verdes ao redor.</t>
+  </si>
+  <si>
+    <t>Natal - RN</t>
+  </si>
+  <si>
+    <t>https://source.unsplash.com/random/560x400/?Natal+RN;https://source.unsplash.com/random/560x400/?Natal+RN;https://source.unsplash.com/random/560x400/?Natal+RN;</t>
+  </si>
+  <si>
+    <t>Natal é a capital do estado do Rio Grande do Norte, localizada na região nordeste do Brasil. Conhecida como a "Cidade do Sol", é um destino turístico popular devido às suas belas praias, clima tropical e cultura vibrante. Além de suas praias deslumbrantes, Natal oferece uma mistura encantadora de história, gastronomia, artesanato local e festividades tradicionais. Com uma atmosfera descontraída e acolhedora, a cidade é perfeita para quem busca relaxamento à beira-mar, esportes aquáticos emocionantes e uma imersão na cultura nordestina.</t>
+  </si>
+  <si>
+    <t>Praia de Ponta Negra: Considerada uma das praias mais famosas de Natal, Ponta Negra é um verdadeiro paraíso tropical;Forte dos Reis Magos: Localizado na foz do Rio Potengi, o Forte dos Reis Magos é uma fortaleza histórica que remonta ao século XVI;Centro Histórico de Natal: O Centro Histórico abriga belos edifícios coloniais, igrejas centenárias e praças encantadoras;Parque das Dunas: O Parque das Dunas é uma área de preservação ambiental que oferece uma experiência única de contato com a natureza.</t>
+  </si>
+  <si>
+    <t>Ônibus: O transporte público de ônibus é uma opção conveniente para se deslocar dentro de Natal e para as praias próximas. A cidade possui um sistema de transporte eficiente, com diversas linhas que cobrem os principais pontos turísticos;Táxi e transporte por aplicativo: Táxis e serviços de transporte por aplicativo, como Uber e 99, estão disponíveis em Natal. São opções práticas para viagens mais curtas ou para se deslocar com mais conforto e conveniência;Aluguel de carro: Para explorar a região com mais autonomia, é possível alugar um carro em Natal. Isso permite maior flexibilidade para visitar diferentes praias, atrações e destinos turísticos nos arredores da cidade;Bicicleta: Natal possui ciclovias em algumas áreas, sendo uma opção agradável para explorar determinadas regiões da cidade, como a orla marítima. Algumas empresas e pontos turísticos também oferecem aluguel de bicicletas para os visitantes;Caminhadas: Em algumas áreas centrais de Natal, como a Praia de Ponta Negra e o Centro Histórico, é possível explorar a pé. Caminhar pela praia, calçadões e ruas pitorescas é uma maneira agradável de apreciar a cidade e descobrir suas atrações turísticas.</t>
+  </si>
+  <si>
+    <t>Belém - PA</t>
+  </si>
+  <si>
+    <t>https://source.unsplash.com/random/560x400/?Belém+PA;https://source.unsplash.com/random/560x400/?Belém+PA;https://source.unsplash.com/random/560x400/?Belém+PA;</t>
+  </si>
+  <si>
+    <t>Belém é a capital do estado do Pará, localizada na região norte do Brasil. Conhecida como a "Cidade das Mangueiras", é uma cidade rica em história, cultura e belezas naturais. Com sua localização privilegiada às margens do Rio Guamá e próxima à Floresta Amazônica, Belém oferece uma experiência única aos turistas que desejam conhecer a Amazônia brasileira. Além disso, a cidade é famosa por sua gastronomia rica em sabores regionais, artesanato tradicional e festivais culturais.</t>
+  </si>
+  <si>
+    <t>Complexo Feliz Lusitânia: O Complexo Feliz Lusitânia é um conjunto de construções históricas localizadas no centro de Belém;Mercado Ver-o-Peso: Considerado um dos maiores mercados ao ar livre da América Latina, o Mercado Ver-o-Peso é uma atração imperdível em Belém;Mangal das Garças: Localizado às margens do Rio Guamá, o Mangal das Garças é um santuário ecológico que preserva a flora e a fauna da região;Ilha do Combu: A Ilha do Combu é um refúgio de tranquilidade e natureza em meio à agitação da cidade.</t>
+  </si>
+  <si>
+    <t>Barco: Belém é uma cidade cortada por rios, sendo o transporte fluvial uma opção interessante para conhecer a região. Há barcos que fazem travessias para as ilhas próximas, como a Ilha do Combu, e também oferecem passeios pelos rios da região, proporcionando uma experiência única na Amazônia;Ônibus: O sistema de transporte público de Belém conta com linhas de ônibus que conectam os principais pontos da cidade e também permitem o deslocamento para municípios vizinhos. É uma opção econômica e prática para se locomover pela cidade e explorar suas atrações turísticas;Táxi e transporte por aplicativo: Táxis e serviços de transporte por aplicativo, como Uber e 99, estão disponíveis em Belém. São opções convenientes para viagens mais curtas ou para se deslocar com mais conforto e privacidade;Bicicleta: Belém possui ciclovias e ciclofaixas em algumas áreas da cidade, proporcionando uma alternativa sustentável e saudável de locomoção. É possível alugar bicicletas em alguns pontos da cidade ou utilizar aplicativos de compartilhamento de bicicletas para explorar os arredores;Caminhadas: Belém possui áreas centrais que são propícias para caminhadas, como a região do Complexo Feliz Lusitânia e o entorno da Estação das Docas. Caminhar pela cidade é uma ótima maneira de apreciar a arquitetura histórica, descobrir ruas charmosas, visitar mercados e interagir com a cultura local.</t>
+  </si>
+  <si>
+    <t>São Luís - MA</t>
+  </si>
+  <si>
+    <t>São Luís é a capital do estado do Maranhão, localizada na região nordeste do Brasil. Com sua rica herança cultural e arquitetônica, a cidade encanta os visitantes com sua atmosfera histórica e beleza única. Reconhecida como Patrimônio Mundial da Humanidade pela UNESCO, São Luís preserva um conjunto arquitetônico colonial que reflete a influência portuguesa, africana e indígena em sua história. Além disso, a cidade é famosa pelo seu folclore, culinária típica e praias paradisíacas.</t>
+  </si>
+  <si>
+    <t>Centro Histórico: O centro histórico de São Luís é um dos principais atrativos da cidade;Lençóis Maranhenses: A cerca de 250 km de São Luís, encontra-se o Parque Nacional dos Lençóis Maranhenses, uma verdadeira maravilha natural;Praia de São Marcos: Localizada na área urbana de São Luís, a Praia de São Marcos é uma das principais praias da cidade;Centro Cultural da Vale: O Centro Cultural da Vale é um espaço cultural que abriga exposições, apresentações artísticas e eventos em São Luís.</t>
+  </si>
+  <si>
+    <t>Ônibus: O sistema de transporte público de São Luís é composto por ônibus que percorrem diferentes partes da cidade. É uma opção econômica para se deslocar pelos bairros e visitar os pontos turísticos;Táxi e transporte por aplicativo: Táxis e serviços de transporte por aplicativo, como Uber e 99, estão disponíveis em São Luís. São alternativas práticas e convenientes para viagens mais curtas ou para explorar a cidade com maior conforto;Caminhadas: Em muitas áreas do centro histórico de São Luís, é possível explorar a pé. Caminhar pelas ruas estreitas e admirar a arquitetura colonial é uma experiência encantadora;Aluguel de carro: Para explorar a região além de São Luís, como os Lençóis Maranhenses, o aluguel de carro pode ser uma opção interessante. Isso permite maior autonomia e flexibilidade</t>
+  </si>
+  <si>
+    <t>Belo Horizonte - MG</t>
+  </si>
+  <si>
+    <t>Belo Horizonte é a capital do estado de Minas Gerais, localizada na região sudeste do Brasil. Conhecida por sua arquitetura moderna, vida cultural vibrante e gastronomia diversificada, a cidade oferece uma experiência única aos visitantes. Com seu clima agradável, belas paisagens e uma rica história, Belo Horizonte é um destino turístico cada vez mais procurado.</t>
+  </si>
+  <si>
+    <t>Praça da Liberdade: A Praça da Liberdade é um dos principais cartões-postais de Belo Horizonte;Mercado Central: O Mercado Central de Belo Horizonte é um verdadeiro paraíso para os amantes da gastronomia e da cultura local;Pampulha: A região da Pampulha é um importante conjunto arquitetônico e paisagístico de Belo Horizonte;Inhotim: Embora localizado na cidade vizinha de Brumadinho, Inhotim é um destino imperdível para quem visita Belo Horizonte.</t>
+  </si>
+  <si>
+    <t>https://source.unsplash.com/random/560x400/?Belo+Horizonte+MG;https://source.unsplash.com/random/560x400/?Belo+Horizonte+MG;https://source.unsplash.com/random/560x400/?Belo+Horizonte+MG;</t>
+  </si>
+  <si>
+    <t>https://source.unsplash.com/random/560x400/?São+Luis+MA;https://source.unsplash.com/random/560x400/?São+Luis+MA;https://source.unsplash.com/random/560x400/?São+Luis+MA;</t>
+  </si>
+  <si>
+    <t>Ônibus: Belo Horizonte possui um sistema de transporte público bem desenvolvido, com uma ampla rede de ônibus que cobre toda a cidade. É uma opção econômica e conveniente para se deslocar pelos bairros e visitar os pontos turísticos;Metrô: A cidade também conta com um sistema de metrô, que conecta diversas regiões de Belo Horizonte. É uma opção rápida e eficiente para se locomover, principalmente em trajetos mais longos;Táxi e transporte por aplicativo: Táxis e serviços de transporte por aplicativo, como Uber e 99, estão disponíveis em Belo Horizonte. São opções práticas para viagens mais curtas ou para quem deseja mais comodidade e conforto;Caminhadas: Em algumas áreas da cidade, especialmente no centro histórico e em regiões com maior concentração de atrações turísticas, é possível explorar Belo Horizonte a pé. Caminhar pelas ruas e praças é uma forma agradável de apreciar a arquitetura, descobrir lugares interessantes e vivenciar a atmosfera local;Aluguel de bicicletas: Belo Horizonte possui um sistema de aluguel de bicicletas compartilhadas, conhecido como "Bike BH". É uma opção saudável e sustentável para se locomover pela cidade, especialmente em áreas com ciclovias e ciclofaixas.</t>
+  </si>
+  <si>
+    <t>Recife - PE</t>
+  </si>
+  <si>
+    <t>https://source.unsplash.com/random/560x400/?Recife+PE;https://source.unsplash.com/random/560x400/?Recife+PE;https://source.unsplash.com/random/560x400/?Recife+PE;</t>
+  </si>
+  <si>
+    <t>Recife é a capital do estado de Pernambuco, situada na região nordeste do Brasil. Conhecida como a "Veneza Brasileira" devido aos seus rios, pontes e canais, a cidade oferece uma mistura encantadora de história, cultura, praias deslumbrantes e uma animada cena cultural. Com sua arquitetura colonial, rica herança afro-brasileira e festividades populares, Recife encanta visitantes de todo o mundo.</t>
+  </si>
+  <si>
+    <t>Recife Antigo: O bairro do Recife Antigo é o centro histórico da cidade e um dos principais pontos turísticos;Praia de Boa Viagem: Considerada uma das mais famosas praias urbanas do Brasil, a Praia de Boa Viagem é um verdadeiro cartão-postal de Recife;Instituto Ricardo Brennand: Localizado nos arredores de Recife, o Instituto Ricardo Brennand é um complexo cultural e museu imperdível para os amantes de arte e história;Olinda: Embora não seja uma cidade independente, Olinda é uma cidade vizinha de Recife e um destino turístico muito popular.</t>
+  </si>
+  <si>
+    <t>Ônibus: Recife possui um sistema de transporte público abrangente, com linhas de ônibus que atendem a toda a cidade e seus arredores. É uma opção econômica para se deslocar pelos bairros e visitar os pontos turísticos;Metrô: A cidade conta com um sistema de metrô que conecta diferentes partes de Recife e sua região metropolitana. É uma opção rápida e eficiente para se locomover, especialmente em trajetos mais longos;Táxi e transporte por aplicativo: Táxis e serviços de transporte por aplicativo, como Uber e 99, estão disponíveis em Recife. São opções convenientes para viagens mais curtas ou para quem deseja mais conforto e comodidade;Caminhadas: Em muitas áreas do Recife Antigo e de outros bairros turísticos, é possível explorar a cidade a pé. Caminhar pelas ruas e becos é uma forma agradável de apreciar a arquitetura histórica, descobrir detalhes encantadores e vivenciar a atmosfera local.</t>
+  </si>
+  <si>
+    <t>Brasília - DF</t>
+  </si>
+  <si>
+    <t>https://source.unsplash.com/random/560x400/?Brasília+DF;https://source.unsplash.com/random/560x400/?Brasília+DF;https://source.unsplash.com/random/560x400/?Brasília+DF;</t>
+  </si>
+  <si>
+    <t>Brasília é a capital do Brasil e está localizada no Distrito Federal, no coração do país. Projetada pelo renomado arquiteto Oscar Niemeyer e pelo urbanista Lúcio Costa, a cidade é conhecida mundialmente por sua arquitetura moderna e planejamento urbano único. Além de ser a sede do governo brasileiro, Brasília também oferece uma série de atrações turísticas que encantam os visitantes.</t>
+  </si>
+  <si>
+    <t>Esplanada dos Ministérios: A Esplanada dos Ministérios é um dos principais cartões-postais de Brasília;Catedral Metropolitana: Projetada por Oscar Niemeyer, a Catedral Metropolitana de Brasília é uma obra-prima da arquitetura;Palácio da Alvorada: A residência oficial do presidente do Brasil, o Palácio da Alvorada, também é um ponto turístico importante em Brasília;Pontão do Lago Sul: Localizado às margens do Lago Paranoá, o Pontão do Lago Sul é um complexo de entretenimento e lazer.</t>
+  </si>
+  <si>
+    <t>Ônibus: Brasília possui um sistema de transporte público bem estruturado, com linhas de ônibus que percorrem toda a cidade. É uma opção acessível para se deslocar entre os pontos turísticos e explorar diferentes áreas da capital;Metrô: A cidade conta com um sistema de metrô que conecta diversas regiões, incluindo o Aeroporto Internacional de Brasília. É uma opção conveniente e eficiente para se locomover, especialmente em trajetos mais longos;Táxi e transporte por aplicativo: Táxis e serviços de transporte por aplicativo, como Uber e 99, estão disponíveis em Brasília. São opções práticas para viagens mais curtas ou para quem deseja mais comodidade e conforto;Aluguel de carro: Para quem prefere ter mais autonomia e flexibilidade durante a estadia em Brasília, o aluguel de carro é uma alternativa viável. A cidade possui boas vias e estacionamentos, o que facilita a locomoção e permite explorar os arredores com facilidade.</t>
+  </si>
+  <si>
+    <t>Porto Alegre - MS</t>
+  </si>
+  <si>
+    <t>https://source.unsplash.com/random/560x400/?Porto+Alegre+MS;https://source.unsplash.com/random/560x400/?Porto+Alegre+MS;https://source.unsplash.com/random/560x400/?Porto+Alegre+MS;</t>
+  </si>
+  <si>
+    <t>Porto Alegre é a capital do estado do Rio Grande do Sul e uma cidade que mescla modernidade e tradição. Localizada na região Sul do Brasil, é conhecida por sua cultura gaúcha, rica gastronomia, parques e uma vida cultural vibrante. Com uma atmosfera acolhedora, Porto Alegre encanta seus visitantes com suas paisagens, arquitetura histórica e diversas opções de lazer.</t>
+  </si>
+  <si>
+    <t>Centro Histórico: O Centro Histórico de Porto Alegre é um verdadeiro tesouro para os amantes de história;Parque da Redenção: Também conhecido como Parque Farroupilha, o Parque da Redenção é uma área verde de 37 hectares no coração da cidade;Orla do Guaíba: A Orla do Guaíba é um dos principais cartões-postais de Porto Alegre. Localizada às margens do Rio Guaíba, oferece uma vista deslumbrante e é perfeita para apreciar o pôr do sol;Museu de Arte do Rio Grande do Sul (MARGS): O MARGS é um importante museu de arte contemporânea e moderna em Porto Alegre.</t>
+  </si>
+  <si>
+    <t>Ônibus: Porto Alegre possui um sistema de transporte público bem desenvolvido, com uma extensa rede de ônibus que cobre toda a cidade. É uma opção econômica e prática para se deslocar pelos diferentes bairros e visitar os pontos turísticos;Metrô: A cidade não possui sistema de metrô, mas há projetos em andamento para a construção de uma linha de metrô. No momento, o transporte ferroviário é utilizado para trajetos intermunicipais;Táxi e transporte por aplicativo: Táxis e serviços de transporte por aplicativo, como Uber e 99, estão disponíveis em Porto Alegre. São opções convenientes para viagens mais curtas ou para quem deseja mais conforto e comodidade;Caminhadas: Porto Alegre é uma cidade que pode ser explorada a pé em muitas áreas, especialmente no centro histórico</t>
+  </si>
+  <si>
+    <t>João Pessoa - PB</t>
+  </si>
+  <si>
+    <t>João Pessoa é a capital do estado da Paraíba e uma cidade repleta de encantos naturais e cultura rica. Localizada no extremo leste do país, é conhecida por suas belas praias, riqueza histórica e estilo de vida tranquilo. Com um clima tropical e uma população acolhedora, João Pessoa oferece aos visitantes um ambiente relaxante e muitas opções de lazer.</t>
+  </si>
+  <si>
+    <t>https://source.unsplash.com/random/560x400/?joao+pessoa+PB;https://source.unsplash.com/random/560x400/?joao+pessoa+PB;https://source.unsplash.com/random/560x400/?joao+pessoa+PB;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Praia de Tambaú: Uma das praias mais famosas de João Pessoa, Tambaú é conhecida por suas águas calmas e clara;Centro Histórico: O Centro Histórico de João Pessoa é uma verdadeira viagem ao passado;Farol do Cabo Branco: Localizado no ponto mais oriental das Américas, o Farol do Cabo Branco é um marco importante em João Pessoa;Estação Cabo Branco - Ciência, Cultura e Artes: Projetada por Oscar Niemeyer, a Estação Cabo Branco é um espaço cultural que combina ciência, arte e arquitetura moderna. </t>
+  </si>
+  <si>
+    <t>Ônibus: João Pessoa possui um sistema de transporte público eficiente, com diversas linhas de ônibus que atendem a cidade. É uma opção econômica para se deslocar pelos bairros e visitar os pontos turísticos;Táxi e transporte por aplicativo: Táxis e serviços de transporte por aplicativo, como Uber e 99, estão disponíveis em João Pessoa. São opções práticas e convenientes, especialmente para trajetos mais curtos ou para quem deseja mais conforto e comodidade;Bicicleta: A cidade conta com um sistema de aluguel de bicicletas chamado "Bike JP". É uma forma saudável e sustentável de explorar João Pessoa, principalmente em áreas mais próximas das praias e do centro;Carro alugado: Para quem deseja ter mais autonomia e flexibilidade durante a estadia em João Pessoa, o aluguel de carro é uma opção viável. A cidade possui boas vias e estacionamentos, o que facilita a locomoção de carro. No entanto, é importante estar atento ao trânsito e seguir as regras de estacionamento.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -146,6 +402,12 @@
       <name val="Söhne"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF374151"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -169,7 +431,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -180,16 +442,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -202,6 +458,19 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hiperlink" xfId="2" builtinId="8"/>
@@ -520,9 +789,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K99"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -531,7 +800,8 @@
     <col min="2" max="2" width="24.28515625" style="2" customWidth="1"/>
     <col min="3" max="3" width="55.140625" style="2" customWidth="1"/>
     <col min="4" max="5" width="41.7109375" style="2" customWidth="1"/>
-    <col min="6" max="10" width="41.28515625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="63.85546875" style="2" customWidth="1"/>
+    <col min="7" max="10" width="41.28515625" style="2" customWidth="1"/>
     <col min="11" max="11" width="24" style="2" customWidth="1"/>
     <col min="12" max="16384" width="9.140625" style="2"/>
   </cols>
@@ -540,19 +810,19 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="1"/>
@@ -561,34 +831,34 @@
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
     </row>
-    <row r="2" spans="1:11" ht="345">
+    <row r="2" spans="1:11" ht="225">
       <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="330">
+    <row r="3" spans="1:11" ht="210">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="8" t="s">
         <v>19</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -601,17 +871,17 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="360">
+    <row r="4" spans="1:11" ht="240">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="7" t="s">
         <v>16</v>
       </c>
       <c r="E4" s="2" t="s">
@@ -622,66 +892,358 @@
       </c>
     </row>
     <row r="5" spans="1:11" ht="87.75" customHeight="1">
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-    </row>
-    <row r="6" spans="1:11" ht="87" customHeight="1"/>
-    <row r="7" spans="1:11">
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-    </row>
-    <row r="9" spans="1:11">
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-    </row>
-    <row r="11" spans="1:11">
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-    </row>
-    <row r="13" spans="1:11">
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-    </row>
-    <row r="14" spans="1:11">
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
-    </row>
-    <row r="15" spans="1:11">
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-    </row>
-    <row r="17" spans="2:3">
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-    </row>
-    <row r="19" spans="2:3">
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-    </row>
-    <row r="21" spans="2:3">
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-    </row>
-    <row r="23" spans="2:3">
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-    </row>
-    <row r="25" spans="2:3">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="135.75" customHeight="1">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="144.75" customHeight="1">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="122.25" customHeight="1">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="99" customHeight="1">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="142.5" customHeight="1">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="144.75" customHeight="1">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="114" customHeight="1">
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="135.75" customHeight="1">
+      <c r="A13" s="2">
+        <v>12</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="124.5" customHeight="1">
+      <c r="A14" s="2">
+        <v>13</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="120" customHeight="1">
+      <c r="A15" s="2">
+        <v>14</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="146.25" customHeight="1">
+      <c r="A16" s="2">
+        <v>15</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="141" customHeight="1">
+      <c r="A17" s="2">
+        <v>16</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="132" customHeight="1">
+      <c r="A18" s="2">
+        <v>17</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="125.25" customHeight="1">
+      <c r="A19" s="2">
+        <v>18</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F19" s="14" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="138" customHeight="1">
+      <c r="A20" s="2">
+        <v>19</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="120.75" customHeight="1">
+      <c r="A21" s="2">
+        <v>20</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
     </row>
-    <row r="27" spans="2:3">
+    <row r="27" spans="1:6">
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
     </row>
-    <row r="29" spans="2:3">
+    <row r="29" spans="1:6">
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
     </row>
-    <row r="31" spans="2:3">
+    <row r="31" spans="1:6">
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
     </row>
@@ -826,7 +1388,25 @@
     <hyperlink ref="C2" r:id="rId1" xr:uid="{5FC5D7BE-92F8-4ED1-805C-33C9F1254D39}"/>
     <hyperlink ref="C3" r:id="rId2" xr:uid="{F58687A4-207C-47D4-8572-938C7436D3F7}"/>
     <hyperlink ref="C4" r:id="rId3" xr:uid="{421BC998-1404-423A-B886-62923E2C2D12}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{40458A8D-47F7-4F69-9551-240590638975}"/>
+    <hyperlink ref="C6" r:id="rId5" xr:uid="{9277AB53-7DCC-456D-9C00-0777AF5A53D2}"/>
+    <hyperlink ref="C7" r:id="rId6" xr:uid="{14C3043B-0E33-4CFE-8F30-6970283AB789}"/>
+    <hyperlink ref="C8" r:id="rId7" xr:uid="{73947CE4-0A6A-49CF-AE03-B2A5A81E95D1}"/>
+    <hyperlink ref="C9" r:id="rId8" xr:uid="{89603598-BC3C-4AD6-84DC-10701C22037A}"/>
+    <hyperlink ref="C10" r:id="rId9" xr:uid="{74A0489E-3312-4BBE-A6C0-CEB98527AFAD}"/>
+    <hyperlink ref="C11" r:id="rId10" xr:uid="{458EE7BB-006C-4847-BDDF-028CA53BAC96}"/>
+    <hyperlink ref="C12" r:id="rId11" xr:uid="{FCDA8258-8DE7-46ED-B1AD-122435C8E2F1}"/>
+    <hyperlink ref="C13" r:id="rId12" xr:uid="{706622DA-14B7-4B5E-BF84-14BE980341B3}"/>
+    <hyperlink ref="C14" r:id="rId13" xr:uid="{3F2BBE57-F43F-4A68-943D-790FA49706CC}"/>
+    <hyperlink ref="C15" r:id="rId14" xr:uid="{05326A5C-180D-4FFD-95E7-EB1DE5D0137A}"/>
+    <hyperlink ref="C16" r:id="rId15" xr:uid="{3C82BD82-0C62-4F58-A782-F1DAFF8788BD}"/>
+    <hyperlink ref="C17" r:id="rId16" xr:uid="{B759624C-793E-499D-B47E-C86498B4F2FE}"/>
+    <hyperlink ref="C18" r:id="rId17" xr:uid="{8D7D41F0-B149-4148-90A4-FA1B05256496}"/>
+    <hyperlink ref="C19" r:id="rId18" xr:uid="{52B919C8-F223-4CFF-9DE9-C8C729B72341}"/>
+    <hyperlink ref="C20" r:id="rId19" xr:uid="{026AABD1-FF1B-4DA9-9372-281154D4772F}"/>
+    <hyperlink ref="C21" r:id="rId20" xr:uid="{3616FCB2-7F41-48C0-B7F5-E294050B47BB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId21"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Feat: fotos de lugares adicionadas
</commit_message>
<xml_diff>
--- a/assets/xlsx/locais.xlsx
+++ b/assets/xlsx/locais.xlsx
@@ -40,7 +40,7 @@
     <t>Rio de Janeiro - RIO DE JANEIRO</t>
   </si>
   <si>
-    <t>\assets\images\pontos-tur\rio-de-janeiro.jpg ; \assets\images\pontos-tur\rio-de-janeiro2.jpg ; \assets\images\pontos-tur\rio-de-janeiro3.jpg</t>
+    <t>\assets\images\pontos-tur\rio-de-janeiro.jpg ; \assets\images\pontos-tur\rio-de-janeiro2.jpg ; \assets\images\pontos-tur\rio-de-janeiro3.jpg ; \assets\images\Locais\rio-capa.jpg</t>
   </si>
   <si>
     <t>O Rio de Janeiro é uma cidade mundialmente conhecida por suas praias incríveis, vistas deslumbrantes e vida noturna animada. &amp;#10;&amp;#10;Além disso, a cidade oferece uma rica cultura, com destaque para a música, dança e gastronomia. O turismo é uma das principais atividades econômicas da cidade, atraindo milhões de visitantes todos os anos.</t>
@@ -58,7 +58,7 @@
     <t>Salvador - BAHIA</t>
   </si>
   <si>
-    <t xml:space="preserve">\assets\images\Locais\salvador1.jpg ;&amp;#10;\assets\images\Locais\salvador2.jpg ; \assets\images\Locais\salvador3.jpg </t>
+    <t>\assets\images\Locais\salvador1.jpg ;\assets\images\Locais\salvador2.jpg ; \assets\images\Locais\salvador3.jpg ; \assets\images\Locais\salvador-capa.jpg</t>
   </si>
   <si>
     <t>Salvador é uma cidade vibrante e encantadora localizada na região nordeste do Brasil. Conhecida por sua rica cultura, arquitetura histórica e praias deslumbrantes, a cidade atrai milhões de turistas todos os anos. Com uma mistura única de influências africanas, indígenas e europeias, Salvador oferece uma experiência cultural rica e diversificada.</t>
@@ -76,7 +76,7 @@
     <t>Florianópolis - SANTA CATARINA</t>
   </si>
   <si>
-    <t>\assets\images\Locais\florianopolis1.jpg;&amp;#10;\assets\images\Locais\florianopolis2.jpg;&amp;#10;\assets\images\Locais\florianopolis3.jpg</t>
+    <t>\assets\images\Locais\florianopolis1.jpg;\assets\images\Locais\florianopolis2.jpg;\assets\images\Locais\florianopolis3.jpg ; \assets\images\Locais\florianopolis-capa.jpg</t>
   </si>
   <si>
     <t>Florianópolis, também conhecida como "Ilha da Magia", é uma cidade encantadora localizada no estado de Santa Catarina, no sul do Brasil. Com suas praias paradisíacas, paisagens deslumbrantes e atmosfera descontraída, é um destino turístico popular tanto para os brasileiros quanto para os estrangeiros. A cidade combina o melhor de uma metrópole moderna com a tranquilidade de uma ilha paradisíaca, oferecendo uma experiência única para os visitantes.</t>
@@ -94,7 +94,7 @@
     <t xml:space="preserve"> Gramado - RIO GRANDE DO SUL</t>
   </si>
   <si>
-    <t>\assets\images\Locais\gramado.jpg;&amp;#10;\assets\images\Locais\gramado1.webp;&amp;#10;\assets\images\Locais\gramado2.jpg</t>
+    <t>\assets\images\Locais\gramado.jpg;\assets\images\Locais\gramado1.webp;\assets\images\Locais\gramado2.jpg ; assets\images\Locais\gramado-capa.jpg</t>
   </si>
   <si>
     <t>Gramado é uma encantadora cidade localizada na Serra Gaúcha, no estado do Rio Grande do Sul. Conhecida por sua atmosfera europeia, paisagens deslumbrantes e clima ameno, é um destino turístico popular no Brasil. Com sua arquitetura charmosa, culinária deliciosa e uma série de atrações, Gramado oferece uma experiência única aos seus visitantes.</t>
@@ -112,7 +112,7 @@
     <t>Bonito - MATO GROSSO DO SUL</t>
   </si>
   <si>
-    <t>https://source.unsplash.com/random/560x400/?Bonito+MS;https://source.unsplash.com/random/560x400/?Bonito+MS;https://source.unsplash.com/random/560x400/?Bonito+MS;</t>
+    <t>\assets\images\Locais\bonito1.jpg ; \assets\images\Locais\bonito2.JPG ; \assets\images\Locais\bonito3.JPG ; \assets\images\Locais\bonito-capa.webp</t>
   </si>
   <si>
     <t>Bonito é um verdadeiro paraíso natural localizado no estado do Mato Grosso do Sul, no Brasil. Conhecida por suas águas cristalinas, rios, cavernas e uma rica diversidade de fauna e flora, a cidade atrai turistas de todo o mundo em busca de aventura e contato com a natureza. Com uma infraestrutura bem desenvolvida para o ecoturismo, Bonito oferece experiências únicas e preservadas para os amantes da natureza.&amp;#10;</t>
@@ -130,7 +130,7 @@
     <t xml:space="preserve"> Paraty - RIO DE JANEIRO</t>
   </si>
   <si>
-    <t>https://source.unsplash.com/random/560x400/?Paraty+RJ;https://source.unsplash.com/random/560x400/?Paraty+RJ;https://source.unsplash.com/random/560x400/?Paraty+RJ;</t>
+    <t>\assets\images\Locais\paraty1.jpg ; \assets\images\Locais\paraty2.jpg ; \assets\images\Locais\paraty3.jpg ; \assets\images\Locais\paraty-capa.jpg</t>
   </si>
   <si>
     <t>Paraty é uma charmosa cidade histórica localizada no estado do Rio de Janeiro, no Brasil. Com sua arquitetura colonial preservada, ruas de pedra e localização privilegiada entre a serra e o mar, Paraty encanta os visitantes com seu clima tranquilo e suas belezas naturais. Além do patrimônio histórico, a cidade também é conhecida por suas praias paradisíacas e pela vasta oferta de passeios de barco e trilhas.</t>
@@ -145,7 +145,7 @@
     <t>Manaus - AMAZONAS</t>
   </si>
   <si>
-    <t>https://source.unsplash.com/random/560x400/?Manaus+AM;https://source.unsplash.com/random/560x400/?Manaus+AM;https://source.unsplash.com/random/560x400/?Manaus+AM;</t>
+    <t>\assets\images\Locais\manaus1.jpg ; \assets\images\Locais\manaus2.jpg ; \assets\images\Locais\manaus3.jpg ; \assets\images\Locais\manaus-capa.webp</t>
   </si>
   <si>
     <t>Manaus, a capital do estado do Amazonas, é uma cidade fascinante localizada no coração da Amazônia brasileira. Conhecida por sua biodiversidade, cultura rica e herança histórica, Manaus é o ponto de partida ideal para explorar a maior floresta tropical do mundo. Com seu clima tropical e paisagens deslumbrantes, a cidade oferece uma experiência única aos turistas, que podem mergulhar na natureza exuberante e descobrir a história e a cultura da região.</t>
@@ -163,7 +163,7 @@
     <t xml:space="preserve"> Foz do Iguaçu - PARANÁ</t>
   </si>
   <si>
-    <t>https://source.unsplash.com/random/560x400/?foz+do+Iguaçu+PR;https://source.unsplash.com/random/560x400/?foz+do+Iguaçu+PR;https://source.unsplash.com/random/560x400/?foz+do+Iguaçu+PR;</t>
+    <t>\assets\images\Locais\foz1.jpg ; \assets\images\Locais\foz2.jpg ; \assets\images\Locais\foz3.jpg ; \assets\images\Locais\foz-capa.jpg</t>
   </si>
   <si>
     <t>Foz do Iguaçu, localizada no estado do Paraná, é uma cidade famosa por abrigar uma das mais impressionantes maravilhas naturais do mundo: as Cataratas do Iguaçu. Além das espetaculares quedas d&amp;apos;água, Foz do Iguaçu é uma cidade multicultural, marcada pela diversidade étnica e pela rica biodiversidade da região. Com uma localização estratégica na tríplice fronteira entre Brasil, Paraguai e Argentina, a cidade oferece aos turistas uma experiência única, com paisagens deslumbrantes e atrações imperdíveis.</t>
@@ -181,7 +181,7 @@
     <t>Ouro Preto - MINAS GERAIS</t>
   </si>
   <si>
-    <t>https://source.unsplash.com/random/560x400/?Ouro+Preto+MG;https://source.unsplash.com/random/560x400/?Ouro+Preto+MG;https://source.unsplash.com/random/560x400/?Ouro+Preto+MG;</t>
+    <t>\assets\images\Locais\ouropreto1.jpg ; \assets\images\Locais\ouropreto2.jfif ; \assets\images\Locais\ouropreto3.jpg ; \assets\images\Locais\ouropreto-capa.jpg</t>
   </si>
   <si>
     <t>Ouro Preto é uma cidade histórica localizada no estado de Minas Gerais, no Brasil. Reconhecida como Patrimônio Mundial pela UNESCO, a cidade preserva a rica herança do período colonial brasileiro. Com suas ladeiras de paralelepípedos, igrejas barrocas, museus e paisagens encantadoras, Ouro Preto atrai visitantes de todo o mundo em busca de cultura, história e beleza arquitetônica. Além disso, a cidade é conhecida pela sua vibrante vida estudantil, pois abriga uma importante universidade.</t>
@@ -199,7 +199,7 @@
     <t>Jericoacoara – CEARÁ</t>
   </si>
   <si>
-    <t>https://source.unsplash.com/random/560x400/?Jericoacoara+CE;https://source.unsplash.com/random/560x400/?Jericoacoara+CE;https://source.unsplash.com/random/560x400/?Jericoacoara+CE;</t>
+    <t>\assets\images\Locais\Jericoacoara1.jpg ; \assets\images\Locais\Jericoacoara2.jpg ; \assets\images\Locais\Jericoacoara3.jpg ; \assets\images\Locais\Jericoacoara-capa.jpg</t>
   </si>
   <si>
     <t>Jericoacoara, carinhosamente conhecida como "Jeri", é uma charmosa vila de pescadores localizada no litoral do estado do Ceará, no nordeste do Brasil. Com suas praias paradisíacas, dunas de areia branca, lagoas cristalinas e paisagens deslumbrantes, Jericoacoara é um destino turístico popular, atraindo visitantes em busca de relaxamento, aventura e contato com a natureza. Além de suas belezas naturais, Jeri oferece uma atmosfera descontraída, com ruas de areia, restaurantes aconchegantes, lojinhas de artesanato e uma vida noturna animada.</t>
@@ -217,7 +217,7 @@
     <t>Olinda- PERNAMBUCO</t>
   </si>
   <si>
-    <t>https://source.unsplash.com/random/560x400/?Olinda+PE;https://source.unsplash.com/random/560x400/?Olinda+PE;https://source.unsplash.com/random/560x400/?Olinda+PE;</t>
+    <t>\assets\images\Locais\olinda1.jpg ; \assets\images\Locais\olinda2.jpg ; \assets\images\Locais\olinda3.JPG ; \assets\images\Locais\olinda-capa.jpg</t>
   </si>
   <si>
     <t>Olinda é uma cidade histórica e culturalmente rica localizada no estado de Pernambuco, no nordeste do Brasil. Fundada em 1535, é considerada Patrimônio Cultural da Humanidade pela UNESCO devido ao seu centro histórico bem preservado, casario colorido, igrejas centenárias e festividades populares. Olinda é famosa por suas ruas de paralelepípedos, ladeiras íngremes, manifestações artísticas e pela alegria contagiante de seu povo. É um destino encantador que oferece uma combinação única de história, arte, religião e beleza natural.</t>
@@ -235,7 +235,7 @@
     <t>Curitiba - PARANÁ</t>
   </si>
   <si>
-    <t>https://source.unsplash.com/random/560x400/?Curitiba+PR;https://source.unsplash.com/random/560x400/?Curitiba+PR;https://source.unsplash.com/random/560x400/?Curitiba+PR;</t>
+    <t>\assets\images\Locais\curitiba1.jpg ; \assets\images\Locais\curitiba2.JPG ; \assets\images\Locais\curitiba3.jpg ; \assets\images\Locais\curitiba-capa.jpg</t>
   </si>
   <si>
     <t>Curitiba é a capital do estado do Paraná, localizada na região sul do Brasil. Conhecida por sua qualidade de vida, planejamento urbano e cultura vibrante, a cidade é um destino turístico encantador. Curitiba oferece uma mistura única de natureza exuberante, arquitetura moderna, parques bem cuidados e uma cena cultural diversificada. Com uma infraestrutura eficiente, a cidade é famosa por suas atrações turísticas, gastronomia deliciosa, eventos culturais e o famoso sistema de transporte público.</t>
@@ -250,7 +250,7 @@
     <t>Natal - RIO GRANDE DO NORTE</t>
   </si>
   <si>
-    <t>https://source.unsplash.com/random/560x400/?Natal+RN;https://source.unsplash.com/random/560x400/?Natal+RN;https://source.unsplash.com/random/560x400/?Natal+RN;</t>
+    <t>\assets\images\Locais\natal1.jpg ; \assets\images\Locais\natal2.jpg ; \assets\images\Locais\natal3.jpg ; \assets\images\Locais\natal-capa.webp</t>
   </si>
   <si>
     <t>Natal é a capital do estado do Rio Grande do Norte, localizada na região nordeste do Brasil. Conhecida como a "Cidade do Sol", é um destino turístico popular devido às suas belas praias, clima tropical e cultura vibrante. Além de suas praias deslumbrantes, Natal oferece uma mistura encantadora de história, gastronomia, artesanato local e festividades tradicionais. Com uma atmosfera descontraída e acolhedora, a cidade é perfeita para quem busca relaxamento à beira-mar, esportes aquáticos emocionantes e uma imersão na cultura nordestina.</t>
@@ -268,7 +268,7 @@
     <t>Belém - PARÁ</t>
   </si>
   <si>
-    <t>https://source.unsplash.com/random/560x400/?Belém+PA;https://source.unsplash.com/random/560x400/?Belém+PA;https://source.unsplash.com/random/560x400/?Belém+PA;</t>
+    <t>\assets\images\Locais\belem1.jpg ; \assets\images\Locais\belem2.jpg ; \assets\images\Locais\belem3.webp ; \assets\images\Locais\belem-capa.webp</t>
   </si>
   <si>
     <t>Belém é a capital do estado do Pará, localizada na região norte do Brasil. Conhecida como a "Cidade das Mangueiras", é uma cidade rica em história, cultura e belezas naturais. Com sua localização privilegiada às margens do Rio Guamá e próxima à Floresta Amazônica, Belém oferece uma experiência única aos turistas que desejam conhecer a Amazônia brasileira. Além disso, a cidade é famosa por sua gastronomia rica em sabores regionais, artesanato tradicional e festivais culturais.</t>
@@ -286,7 +286,7 @@
     <t>São Luís - MARANHÃO</t>
   </si>
   <si>
-    <t>https://source.unsplash.com/random/560x400/?São+Luis+MA;https://source.unsplash.com/random/560x400/?São+Luis+MA;https://source.unsplash.com/random/560x400/?São+Luis+MA;</t>
+    <t>\assets\images\Locais\saoluis1.jpg ; \assets\images\Locais\saoluis2.jpg ; \assets\images\Locais\saoluis3.jpg ; \assets\images\Locais\saoluis-capa.jpg</t>
   </si>
   <si>
     <t>São Luís é a capital do estado do Maranhão, localizada na região nordeste do Brasil. Com sua rica herança cultural e arquitetônica, a cidade encanta os visitantes com sua atmosfera histórica e beleza única. Reconhecida como Patrimônio Mundial da Humanidade pela UNESCO, São Luís preserva um conjunto arquitetônico colonial que reflete a influência portuguesa, africana e indígena em sua história. Além disso, a cidade é famosa pelo seu folclore, culinária típica e praias paradisíacas.</t>
@@ -304,7 +304,7 @@
     <t>Belo Horizonte - MINAS GERAIS</t>
   </si>
   <si>
-    <t>https://source.unsplash.com/random/560x400/?Belo+Horizonte+MG;https://source.unsplash.com/random/560x400/?Belo+Horizonte+MG;https://source.unsplash.com/random/560x400/?Belo+Horizonte+MG;</t>
+    <t>\assets\images\Locais\bh1.jpg ; \assets\images\Locais\bh2.jpg ; \assets\images\Locais\bh3.webp ; \assets\images\Locais\bh-capa.jpg</t>
   </si>
   <si>
     <t>Belo Horizonte é a capital do estado de Minas Gerais, localizada na região sudeste do Brasil. Conhecida por sua arquitetura moderna, vida cultural vibrante e gastronomia diversificada, a cidade oferece uma experiência única aos visitantes. Com seu clima agradável, belas paisagens e uma rica história, Belo Horizonte é um destino turístico cada vez mais procurado.</t>
@@ -319,7 +319,7 @@
     <t>Recife - PERNAMBUCO</t>
   </si>
   <si>
-    <t>https://source.unsplash.com/random/560x400/?Recife+PE;https://source.unsplash.com/random/560x400/?Recife+PE;https://source.unsplash.com/random/560x400/?Recife+PE;</t>
+    <t>\assets\images\Locais\recife1.jpg ; \assets\images\Locais\recife3.jfif ; \assets\images\Locais\recife3.webp ; \assets\images\Locais\recife-capa.jpg</t>
   </si>
   <si>
     <t>Recife é a capital do estado de Pernambuco, situada na região nordeste do Brasil. Conhecida como a "Veneza Brasileira" devido aos seus rios, pontes e canais, a cidade oferece uma mistura encantadora de história, cultura, praias deslumbrantes e uma animada cena cultural. Com sua arquitetura colonial, rica herança afro-brasileira e festividades populares, Recife encanta visitantes de todo o mundo.</t>
@@ -334,7 +334,7 @@
     <t>Brasília - DISTRITO FEDERAL</t>
   </si>
   <si>
-    <t>https://source.unsplash.com/random/560x400/?Brasília+DF;https://source.unsplash.com/random/560x400/?Brasília+DF;https://source.unsplash.com/random/560x400/?Brasília+DF;</t>
+    <t>\assets\images\Locais\brasilia1.jfif ; \assets\images\Locais\brasilia1.jpg ; \assets\images\Locais\brasilia2.jpg ; \assets\images\Locais\brasilia-capa.jpg</t>
   </si>
   <si>
     <t>Brasília é a capital do Brasil e está localizada no Distrito Federal, no coração do país. Projetada pelo renomado arquiteto Oscar Niemeyer e pelo urbanista Lúcio Costa, a cidade é conhecida mundialmente por sua arquitetura moderna e planejamento urbano único. Além de ser a sede do governo brasileiro, Brasília também oferece uma série de atrações turísticas que encantam os visitantes.</t>
@@ -352,7 +352,7 @@
     <t>Porto Alegre - RIO GRANDE DO SUL</t>
   </si>
   <si>
-    <t>https://source.unsplash.com/random/560x400/?Porto+Alegre+MS;https://source.unsplash.com/random/560x400/?Porto+Alegre+MS;https://source.unsplash.com/random/560x400/?Porto+Alegre+MS;</t>
+    <t>\assets\images\Locais\portoalegre1.png ; \assets\images\Locais\portoalegre2.jpg ; \assets\images\Locais\portoalegre3.jpg ; \assets\images\Locais\portoalegre-capa.jpg</t>
   </si>
   <si>
     <t>Porto Alegre é a capital do estado do Rio Grande do Sul e uma cidade que mescla modernidade e tradição. Localizada na região Sul do Brasil, é conhecida por sua cultura gaúcha, rica gastronomia, parques e uma vida cultural vibrante. Com uma atmosfera acolhedora, Porto Alegre encanta seus visitantes com suas paisagens, arquitetura histórica e diversas opções de lazer.</t>
@@ -367,7 +367,7 @@
     <t>João Pessoa - PARAÍBA</t>
   </si>
   <si>
-    <t>https://source.unsplash.com/random/560x400/?joao+pessoa+PB;https://source.unsplash.com/random/560x400/?joao+pessoa+PB;https://source.unsplash.com/random/560x400/?joao+pessoa+PB;</t>
+    <t>\assets\images\Locais\joaopessoa1.jpg ; \assets\images\Locais\joaopessoa2.jpg ; \assets\images\Locais\joaopessoa3.jpg ; \assets\images\Locais\joaopessoa-capa.jpg</t>
   </si>
   <si>
     <t>João Pessoa é a capital do estado da Paraíba e uma cidade repleta de encantos naturais e cultura rica. Localizada no extremo leste do país, é conhecida por suas belas praias, riqueza histórica e estilo de vida tranquilo. Com um clima tropical e uma população acolhedora, João Pessoa oferece aos visitantes um ambiente relaxante e muitas opções de lazer.</t>
@@ -384,7 +384,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -424,6 +424,12 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -452,7 +458,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -473,6 +479,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -789,17 +798,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="8" width="9.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="9" width="24.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="9" width="55.14785714285715" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="9" width="41.71928571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="9" width="41.71928571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="9" width="63.86214285714286" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="9" width="26.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="9" width="41.29071428571429" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="9" width="41.29071428571429" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="9" width="41.29071428571429" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="9" width="24.005" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="9" width="9.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="10" width="24.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="10" width="55.14785714285715" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="10" width="41.71928571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="10" width="41.71928571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="10" width="63.86214285714286" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="10" width="26.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="10" width="41.29071428571429" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="10" width="41.29071428571429" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="10" width="41.29071428571429" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="10" width="24.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
@@ -829,7 +838,7 @@
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="45.75">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="44.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -856,7 +865,7 @@
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="33.75">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -883,7 +892,7 @@
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="47.25">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -910,7 +919,7 @@
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="47.25">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -991,7 +1000,7 @@
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="22.5">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="21.75">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -1018,7 +1027,7 @@
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="22.5">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="21.75">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -1045,7 +1054,7 @@
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="22.5">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="21.75">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -1072,7 +1081,7 @@
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="22.5">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="21.75">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -1099,7 +1108,7 @@
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="22.5">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="21.75">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -1126,7 +1135,7 @@
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="22.5">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="21.75">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -1153,7 +1162,7 @@
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="22.5">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="21.75">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -1180,14 +1189,14 @@
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="22.5">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="21.75">
       <c r="A15" s="3">
         <v>14</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="8" t="s">
         <v>84</v>
       </c>
       <c r="D15" s="4" t="s">
@@ -1207,7 +1216,7 @@
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="22.5">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -1234,7 +1243,7 @@
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="22.5">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -1261,7 +1270,7 @@
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -1288,7 +1297,7 @@
       <c r="J18" s="4"/>
       <c r="K18" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="22.5">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -1315,7 +1324,7 @@
       <c r="J19" s="4"/>
       <c r="K19" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -1342,7 +1351,7 @@
       <c r="J20" s="4"/>
       <c r="K20" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -1369,7 +1378,7 @@
       <c r="J21" s="4"/>
       <c r="K21" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
       <c r="A22" s="3"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -1382,7 +1391,7 @@
       <c r="J22" s="4"/>
       <c r="K22" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
       <c r="A23" s="3"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -1395,7 +1404,7 @@
       <c r="J23" s="4"/>
       <c r="K23" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
       <c r="A24" s="3"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -1408,7 +1417,7 @@
       <c r="J24" s="4"/>
       <c r="K24" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
       <c r="A25" s="3"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -1421,7 +1430,7 @@
       <c r="J25" s="4"/>
       <c r="K25" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
       <c r="A26" s="3"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -1434,7 +1443,7 @@
       <c r="J26" s="4"/>
       <c r="K26" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
       <c r="A27" s="3"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
@@ -1447,7 +1456,7 @@
       <c r="J27" s="4"/>
       <c r="K27" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
       <c r="A28" s="3"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -1460,7 +1469,7 @@
       <c r="J28" s="4"/>
       <c r="K28" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
       <c r="A29" s="3"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
@@ -1473,7 +1482,7 @@
       <c r="J29" s="4"/>
       <c r="K29" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
       <c r="A30" s="3"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
@@ -1486,7 +1495,7 @@
       <c r="J30" s="4"/>
       <c r="K30" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
       <c r="A31" s="3"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
@@ -1499,7 +1508,7 @@
       <c r="J31" s="4"/>
       <c r="K31" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
       <c r="A32" s="3"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -1512,7 +1521,7 @@
       <c r="J32" s="4"/>
       <c r="K32" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
       <c r="A33" s="3"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
@@ -1525,7 +1534,7 @@
       <c r="J33" s="4"/>
       <c r="K33" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
       <c r="A34" s="3"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
@@ -1538,7 +1547,7 @@
       <c r="J34" s="4"/>
       <c r="K34" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
       <c r="A35" s="3"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
@@ -1551,7 +1560,7 @@
       <c r="J35" s="4"/>
       <c r="K35" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
       <c r="A36" s="3"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
@@ -1564,7 +1573,7 @@
       <c r="J36" s="4"/>
       <c r="K36" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
       <c r="A37" s="3"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
@@ -1577,7 +1586,7 @@
       <c r="J37" s="4"/>
       <c r="K37" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
       <c r="A38" s="3"/>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
@@ -1590,7 +1599,7 @@
       <c r="J38" s="4"/>
       <c r="K38" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
       <c r="A39" s="3"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
@@ -1603,7 +1612,7 @@
       <c r="J39" s="4"/>
       <c r="K39" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
       <c r="A40" s="3"/>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
@@ -1616,7 +1625,7 @@
       <c r="J40" s="4"/>
       <c r="K40" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75">
       <c r="A41" s="3"/>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
@@ -1629,7 +1638,7 @@
       <c r="J41" s="4"/>
       <c r="K41" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75">
       <c r="A42" s="3"/>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
@@ -1642,7 +1651,7 @@
       <c r="J42" s="4"/>
       <c r="K42" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18.75">
       <c r="A43" s="3"/>
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
@@ -1655,7 +1664,7 @@
       <c r="J43" s="4"/>
       <c r="K43" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18.75">
       <c r="A44" s="3"/>
       <c r="B44" s="4"/>
       <c r="C44" s="4"/>
@@ -1668,7 +1677,7 @@
       <c r="J44" s="4"/>
       <c r="K44" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75">
       <c r="A45" s="3"/>
       <c r="B45" s="4"/>
       <c r="C45" s="4"/>
@@ -1681,7 +1690,7 @@
       <c r="J45" s="4"/>
       <c r="K45" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18.75">
       <c r="A46" s="3"/>
       <c r="B46" s="4"/>
       <c r="C46" s="4"/>
@@ -1694,7 +1703,7 @@
       <c r="J46" s="4"/>
       <c r="K46" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="18.75">
       <c r="A47" s="3"/>
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
@@ -1707,7 +1716,7 @@
       <c r="J47" s="4"/>
       <c r="K47" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="18.75">
       <c r="A48" s="3"/>
       <c r="B48" s="4"/>
       <c r="C48" s="4"/>
@@ -1720,7 +1729,7 @@
       <c r="J48" s="4"/>
       <c r="K48" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="18.75">
       <c r="A49" s="3"/>
       <c r="B49" s="4"/>
       <c r="C49" s="4"/>
@@ -1733,7 +1742,7 @@
       <c r="J49" s="4"/>
       <c r="K49" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="18.75">
       <c r="A50" s="3"/>
       <c r="B50" s="4"/>
       <c r="C50" s="4"/>
@@ -1746,7 +1755,7 @@
       <c r="J50" s="4"/>
       <c r="K50" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="18.75">
       <c r="A51" s="3"/>
       <c r="B51" s="4"/>
       <c r="C51" s="4"/>
@@ -1759,7 +1768,7 @@
       <c r="J51" s="4"/>
       <c r="K51" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="18.75">
       <c r="A52" s="3"/>
       <c r="B52" s="4"/>
       <c r="C52" s="4"/>
@@ -1772,7 +1781,7 @@
       <c r="J52" s="4"/>
       <c r="K52" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="18.75">
       <c r="A53" s="3"/>
       <c r="B53" s="4"/>
       <c r="C53" s="4"/>
@@ -1785,7 +1794,7 @@
       <c r="J53" s="4"/>
       <c r="K53" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="18.75">
       <c r="A54" s="3"/>
       <c r="B54" s="4"/>
       <c r="C54" s="4"/>
@@ -1798,7 +1807,7 @@
       <c r="J54" s="4"/>
       <c r="K54" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="18.75">
       <c r="A55" s="3"/>
       <c r="B55" s="4"/>
       <c r="C55" s="4"/>
@@ -1811,7 +1820,7 @@
       <c r="J55" s="4"/>
       <c r="K55" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="18.75">
       <c r="A56" s="3"/>
       <c r="B56" s="4"/>
       <c r="C56" s="4"/>
@@ -1824,7 +1833,7 @@
       <c r="J56" s="4"/>
       <c r="K56" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="18.75">
       <c r="A57" s="3"/>
       <c r="B57" s="4"/>
       <c r="C57" s="4"/>
@@ -1837,7 +1846,7 @@
       <c r="J57" s="4"/>
       <c r="K57" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="18.75">
       <c r="A58" s="3"/>
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
@@ -1850,7 +1859,7 @@
       <c r="J58" s="4"/>
       <c r="K58" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="18.75">
       <c r="A59" s="3"/>
       <c r="B59" s="4"/>
       <c r="C59" s="4"/>
@@ -1863,7 +1872,7 @@
       <c r="J59" s="4"/>
       <c r="K59" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="18.75">
       <c r="A60" s="3"/>
       <c r="B60" s="4"/>
       <c r="C60" s="4"/>
@@ -1876,7 +1885,7 @@
       <c r="J60" s="4"/>
       <c r="K60" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="18.75">
       <c r="A61" s="3"/>
       <c r="B61" s="4"/>
       <c r="C61" s="4"/>
@@ -1889,7 +1898,7 @@
       <c r="J61" s="4"/>
       <c r="K61" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="18.75">
       <c r="A62" s="3"/>
       <c r="B62" s="4"/>
       <c r="C62" s="4"/>
@@ -1902,7 +1911,7 @@
       <c r="J62" s="4"/>
       <c r="K62" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="18.75">
       <c r="A63" s="3"/>
       <c r="B63" s="4"/>
       <c r="C63" s="4"/>
@@ -1915,7 +1924,7 @@
       <c r="J63" s="4"/>
       <c r="K63" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="18.75">
       <c r="A64" s="3"/>
       <c r="B64" s="4"/>
       <c r="C64" s="4"/>
@@ -1928,7 +1937,7 @@
       <c r="J64" s="4"/>
       <c r="K64" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="18.75">
       <c r="A65" s="3"/>
       <c r="B65" s="4"/>
       <c r="C65" s="4"/>
@@ -1941,7 +1950,7 @@
       <c r="J65" s="4"/>
       <c r="K65" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="18.75">
       <c r="A66" s="3"/>
       <c r="B66" s="4"/>
       <c r="C66" s="4"/>
@@ -1954,7 +1963,7 @@
       <c r="J66" s="4"/>
       <c r="K66" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="18.75">
       <c r="A67" s="3"/>
       <c r="B67" s="4"/>
       <c r="C67" s="4"/>
@@ -1967,7 +1976,7 @@
       <c r="J67" s="4"/>
       <c r="K67" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="18.75">
       <c r="A68" s="3"/>
       <c r="B68" s="4"/>
       <c r="C68" s="4"/>
@@ -1980,7 +1989,7 @@
       <c r="J68" s="4"/>
       <c r="K68" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="18.75">
       <c r="A69" s="3"/>
       <c r="B69" s="4"/>
       <c r="C69" s="4"/>
@@ -1993,7 +2002,7 @@
       <c r="J69" s="4"/>
       <c r="K69" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="18.75">
       <c r="A70" s="3"/>
       <c r="B70" s="4"/>
       <c r="C70" s="4"/>
@@ -2006,7 +2015,7 @@
       <c r="J70" s="4"/>
       <c r="K70" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="18.75">
       <c r="A71" s="3"/>
       <c r="B71" s="4"/>
       <c r="C71" s="4"/>
@@ -2019,7 +2028,7 @@
       <c r="J71" s="4"/>
       <c r="K71" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="18.75">
       <c r="A72" s="3"/>
       <c r="B72" s="4"/>
       <c r="C72" s="4"/>
@@ -2032,7 +2041,7 @@
       <c r="J72" s="4"/>
       <c r="K72" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="18.75">
       <c r="A73" s="3"/>
       <c r="B73" s="4"/>
       <c r="C73" s="4"/>
@@ -2045,7 +2054,7 @@
       <c r="J73" s="4"/>
       <c r="K73" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="18.75">
       <c r="A74" s="3"/>
       <c r="B74" s="4"/>
       <c r="C74" s="4"/>
@@ -2058,7 +2067,7 @@
       <c r="J74" s="4"/>
       <c r="K74" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="18.75">
       <c r="A75" s="3"/>
       <c r="B75" s="4"/>
       <c r="C75" s="4"/>
@@ -2071,7 +2080,7 @@
       <c r="J75" s="4"/>
       <c r="K75" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="18.75">
       <c r="A76" s="3"/>
       <c r="B76" s="4"/>
       <c r="C76" s="4"/>
@@ -2084,7 +2093,7 @@
       <c r="J76" s="4"/>
       <c r="K76" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="18.75">
       <c r="A77" s="3"/>
       <c r="B77" s="4"/>
       <c r="C77" s="4"/>
@@ -2097,7 +2106,7 @@
       <c r="J77" s="4"/>
       <c r="K77" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="18.75">
       <c r="A78" s="3"/>
       <c r="B78" s="4"/>
       <c r="C78" s="4"/>
@@ -2110,7 +2119,7 @@
       <c r="J78" s="4"/>
       <c r="K78" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="18.75">
       <c r="A79" s="3"/>
       <c r="B79" s="4"/>
       <c r="C79" s="4"/>
@@ -2123,7 +2132,7 @@
       <c r="J79" s="4"/>
       <c r="K79" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="18.75">
       <c r="A80" s="3"/>
       <c r="B80" s="4"/>
       <c r="C80" s="4"/>
@@ -2136,7 +2145,7 @@
       <c r="J80" s="4"/>
       <c r="K80" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="18.75">
       <c r="A81" s="3"/>
       <c r="B81" s="4"/>
       <c r="C81" s="4"/>
@@ -2149,7 +2158,7 @@
       <c r="J81" s="4"/>
       <c r="K81" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="18.75">
       <c r="A82" s="3"/>
       <c r="B82" s="4"/>
       <c r="C82" s="4"/>
@@ -2162,7 +2171,7 @@
       <c r="J82" s="4"/>
       <c r="K82" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="18.75">
       <c r="A83" s="3"/>
       <c r="B83" s="4"/>
       <c r="C83" s="4"/>
@@ -2175,7 +2184,7 @@
       <c r="J83" s="4"/>
       <c r="K83" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="18.75">
       <c r="A84" s="3"/>
       <c r="B84" s="4"/>
       <c r="C84" s="4"/>
@@ -2188,7 +2197,7 @@
       <c r="J84" s="4"/>
       <c r="K84" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="18.75">
       <c r="A85" s="3"/>
       <c r="B85" s="4"/>
       <c r="C85" s="4"/>
@@ -2201,7 +2210,7 @@
       <c r="J85" s="4"/>
       <c r="K85" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="18.75">
       <c r="A86" s="3"/>
       <c r="B86" s="4"/>
       <c r="C86" s="4"/>
@@ -2214,7 +2223,7 @@
       <c r="J86" s="4"/>
       <c r="K86" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="18.75">
       <c r="A87" s="3"/>
       <c r="B87" s="4"/>
       <c r="C87" s="4"/>
@@ -2227,7 +2236,7 @@
       <c r="J87" s="4"/>
       <c r="K87" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="18.75">
       <c r="A88" s="3"/>
       <c r="B88" s="4"/>
       <c r="C88" s="4"/>
@@ -2240,7 +2249,7 @@
       <c r="J88" s="4"/>
       <c r="K88" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="18.75">
       <c r="A89" s="3"/>
       <c r="B89" s="4"/>
       <c r="C89" s="4"/>
@@ -2253,7 +2262,7 @@
       <c r="J89" s="4"/>
       <c r="K89" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="18.75">
       <c r="A90" s="3"/>
       <c r="B90" s="4"/>
       <c r="C90" s="4"/>
@@ -2266,7 +2275,7 @@
       <c r="J90" s="4"/>
       <c r="K90" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="18.75">
       <c r="A91" s="3"/>
       <c r="B91" s="4"/>
       <c r="C91" s="4"/>
@@ -2279,7 +2288,7 @@
       <c r="J91" s="4"/>
       <c r="K91" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="18.75">
       <c r="A92" s="3"/>
       <c r="B92" s="4"/>
       <c r="C92" s="4"/>
@@ -2292,7 +2301,7 @@
       <c r="J92" s="4"/>
       <c r="K92" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="18.75">
       <c r="A93" s="3"/>
       <c r="B93" s="4"/>
       <c r="C93" s="4"/>
@@ -2305,7 +2314,7 @@
       <c r="J93" s="4"/>
       <c r="K93" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="18.75">
       <c r="A94" s="3"/>
       <c r="B94" s="4"/>
       <c r="C94" s="4"/>
@@ -2318,7 +2327,7 @@
       <c r="J94" s="4"/>
       <c r="K94" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="18.75">
       <c r="A95" s="3"/>
       <c r="B95" s="4"/>
       <c r="C95" s="4"/>
@@ -2331,7 +2340,7 @@
       <c r="J95" s="4"/>
       <c r="K95" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="18.75">
       <c r="A96" s="3"/>
       <c r="B96" s="4"/>
       <c r="C96" s="4"/>
@@ -2344,7 +2353,7 @@
       <c r="J96" s="4"/>
       <c r="K96" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="18.75">
       <c r="A97" s="3"/>
       <c r="B97" s="4"/>
       <c r="C97" s="4"/>
@@ -2357,7 +2366,7 @@
       <c r="J97" s="4"/>
       <c r="K97" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="18.75">
       <c r="A98" s="3"/>
       <c r="B98" s="4"/>
       <c r="C98" s="4"/>
@@ -2370,7 +2379,7 @@
       <c r="J98" s="4"/>
       <c r="K98" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="99" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="99" customHeight="1" ht="18.75">
       <c r="A99" s="3"/>
       <c r="B99" s="4"/>
       <c r="C99" s="4"/>

</xml_diff>